<commit_message>
fpspreadsheet: Add option to define series labels in TsWorkbookChartSource.
git-svn-id: https://svn.code.sf.net/p/lazarus-ccr/svn@6564 8e941d3f-bd1b-0410-a28a-d453659cc2b4
</commit_message>
<xml_diff>
--- a/components/fpspreadsheet/examples/visual/fpschart/workbookchartsource/test-data.xlsx
+++ b/components/fpspreadsheet/examples/visual/fpschart/workbookchartsource/test-data.xlsx
@@ -1,17 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Prog_Lazarus\svn\lazarus-ccr\components\fpspreadsheet\examples\visual\fpschart\workbookchartsource\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{28B3AEC3-7614-4F7E-B33F-EB2E559673BC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="9525"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="9525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -48,8 +54,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="166" formatCode="0.00000"/>
+    <numFmt numFmtId="168" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,24 +96,37 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -141,9 +164,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -175,9 +198,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -209,9 +250,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -384,16 +443,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -401,272 +460,281 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3">
+        <f>SIN(A2*0.3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>1</v>
       </c>
-      <c r="B2">
-        <f>SIN(A2*0.3)</f>
+      <c r="B3" s="3">
+        <f>SIN(A3*0.3)</f>
         <v>0.29552020666133955</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>2</v>
       </c>
-      <c r="B3">
-        <f t="shared" ref="B3:B31" si="0">SIN(A3*0.3)</f>
+      <c r="B4" s="3">
+        <f t="shared" ref="B4:B32" si="0">SIN(A4*0.3)</f>
         <v>0.56464247339503537</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B5" s="3">
         <f t="shared" si="0"/>
         <v>0.7833269096274833</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B6" s="3">
         <f t="shared" si="0"/>
         <v>0.93203908596722629</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="B7" s="3">
         <f t="shared" si="0"/>
         <v>0.99749498660405445</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
-      <c r="A7">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="B8" s="3">
         <f t="shared" si="0"/>
         <v>0.97384763087819526</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
-      <c r="A8">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>7</v>
       </c>
-      <c r="B8">
+      <c r="B9" s="3">
         <f t="shared" si="0"/>
         <v>0.86320936664887371</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c r="A9">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>8</v>
       </c>
-      <c r="B9">
+      <c r="B10" s="3">
         <f t="shared" si="0"/>
         <v>0.67546318055115095</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>9</v>
       </c>
-      <c r="B10">
+      <c r="B11" s="3">
         <f t="shared" si="0"/>
         <v>0.42737988023383017</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
-      <c r="A11">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>10</v>
       </c>
-      <c r="B11">
+      <c r="B12" s="3">
         <f t="shared" si="0"/>
         <v>0.14112000805986721</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
-      <c r="A12">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>11</v>
       </c>
-      <c r="B12">
+      <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>-0.15774569414324821</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
-      <c r="A13">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>12</v>
       </c>
-      <c r="B13">
+      <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>-0.44252044329485207</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
-      <c r="A14">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
         <v>13</v>
       </c>
-      <c r="B14">
+      <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>-0.68776615918397377</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
-      <c r="A15">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
         <v>14</v>
       </c>
-      <c r="B15">
+      <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>-0.87157577241358819</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
-      <c r="A16">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
         <v>15</v>
       </c>
-      <c r="B16">
+      <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>-0.97753011766509701</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
-      <c r="A17">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
         <v>16</v>
       </c>
-      <c r="B17">
+      <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>-0.99616460883584068</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
-      <c r="A18">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
         <v>17</v>
       </c>
-      <c r="B18">
+      <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>-0.92581468232773245</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
-      <c r="A19">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
         <v>18</v>
       </c>
-      <c r="B19">
+      <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>-0.7727644875559877</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
-      <c r="A20">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
         <v>19</v>
       </c>
-      <c r="B20">
+      <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>-0.55068554259763758</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
-      <c r="A21">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
         <v>20</v>
       </c>
-      <c r="B21">
+      <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>-0.27941549819892586</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
-      <c r="A22">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
         <v>21</v>
       </c>
-      <c r="B22">
+      <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>1.6813900484349713E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
-      <c r="A23">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
         <v>22</v>
       </c>
-      <c r="B23">
+      <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>0.31154136351337786</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
-      <c r="A24">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
         <v>23</v>
       </c>
-      <c r="B24">
+      <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>0.57843976438819944</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
-      <c r="A25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
         <v>24</v>
       </c>
-      <c r="B25">
+      <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>0.79366786384915267</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
-      <c r="A26">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
         <v>25</v>
       </c>
-      <c r="B26">
+      <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>0.9379999767747389</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
-      <c r="A27">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
         <v>26</v>
       </c>
-      <c r="B27">
+      <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>0.99854334537460498</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
-      <c r="A28">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
         <v>27</v>
       </c>
-      <c r="B28">
+      <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>0.9698898108450863</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
-      <c r="A29">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
         <v>28</v>
       </c>
-      <c r="B29">
+      <c r="B30" s="3">
         <f t="shared" si="0"/>
         <v>0.85459890808828043</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
-      <c r="A30">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
         <v>29</v>
       </c>
-      <c r="B30">
+      <c r="B31" s="3">
         <f t="shared" si="0"/>
         <v>0.66296923008218334</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
-      <c r="A31">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
         <v>30</v>
       </c>
-      <c r="B31">
+      <c r="B32" s="3">
         <f t="shared" si="0"/>
         <v>0.41211848524175659</v>
       </c>
@@ -678,16 +746,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -695,227 +761,236 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4">
+        <f t="shared" ref="B2:B27" si="0">COS(A2*0.3)</f>
         <v>1</v>
       </c>
-      <c r="B2">
-        <f>COS(A2*0.3)</f>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4">
+        <f t="shared" si="0"/>
         <v>0.95533648912560598</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>2</v>
       </c>
-      <c r="B3">
-        <f t="shared" ref="B3:B26" si="0">COS(A3*0.3)</f>
+      <c r="B4" s="4">
+        <f t="shared" si="0"/>
         <v>0.82533561490967833</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B5" s="4">
         <f t="shared" si="0"/>
         <v>0.6216099682706645</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B6" s="4">
         <f t="shared" si="0"/>
         <v>0.36235775447667362</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="B7" s="4">
         <f t="shared" si="0"/>
         <v>7.0737201667702906E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
-      <c r="A7">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="B8" s="4">
         <f t="shared" si="0"/>
         <v>-0.22720209469308689</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
-      <c r="A8">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>7</v>
       </c>
-      <c r="B8">
+      <c r="B9" s="4">
         <f t="shared" si="0"/>
         <v>-0.50484610459985757</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c r="A9">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>8</v>
       </c>
-      <c r="B9">
+      <c r="B10" s="4">
         <f t="shared" si="0"/>
         <v>-0.73739371554124544</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>9</v>
       </c>
-      <c r="B10">
+      <c r="B11" s="4">
         <f t="shared" si="0"/>
         <v>-0.90407214201706099</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
-      <c r="A11">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>10</v>
       </c>
-      <c r="B11">
+      <c r="B12" s="4">
         <f t="shared" si="0"/>
         <v>-0.98999249660044542</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
-      <c r="A12">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>11</v>
       </c>
-      <c r="B12">
+      <c r="B13" s="4">
         <f t="shared" si="0"/>
         <v>-0.98747976990886488</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
-      <c r="A13">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>12</v>
       </c>
-      <c r="B13">
+      <c r="B14" s="4">
         <f t="shared" si="0"/>
         <v>-0.89675841633414721</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
-      <c r="A14">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
         <v>13</v>
       </c>
-      <c r="B14">
+      <c r="B15" s="4">
         <f t="shared" si="0"/>
         <v>-0.72593230420014021</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
-      <c r="A15">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
         <v>14</v>
       </c>
-      <c r="B15">
+      <c r="B16" s="4">
         <f t="shared" si="0"/>
         <v>-0.49026082134069943</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
-      <c r="A16">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
         <v>15</v>
       </c>
-      <c r="B16">
+      <c r="B17" s="4">
         <f t="shared" si="0"/>
         <v>-0.2107957994307797</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
-      <c r="A17">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
         <v>16</v>
       </c>
-      <c r="B17">
+      <c r="B18" s="4">
         <f t="shared" si="0"/>
         <v>8.7498983439446398E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
-      <c r="A18">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
         <v>17</v>
       </c>
-      <c r="B18">
+      <c r="B19" s="4">
         <f t="shared" si="0"/>
         <v>0.37797774271298024</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
-      <c r="A19">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
         <v>18</v>
       </c>
-      <c r="B19">
+      <c r="B20" s="4">
         <f t="shared" si="0"/>
         <v>0.63469287594263391</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
-      <c r="A20">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
         <v>19</v>
       </c>
-      <c r="B20">
+      <c r="B21" s="4">
         <f t="shared" si="0"/>
         <v>0.83471278483915978</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
-      <c r="A21">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
         <v>20</v>
       </c>
-      <c r="B21">
+      <c r="B22" s="4">
         <f t="shared" si="0"/>
         <v>0.96017028665036597</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
-      <c r="A22">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
         <v>21</v>
       </c>
-      <c r="B22">
+      <c r="B23" s="4">
         <f t="shared" si="0"/>
         <v>0.9998586363834151</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
-      <c r="A23">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
         <v>22</v>
       </c>
-      <c r="B23">
+      <c r="B24" s="4">
         <f t="shared" si="0"/>
         <v>0.9502325919585296</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
-      <c r="A24">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
         <v>23</v>
       </c>
-      <c r="B24">
+      <c r="B25" s="4">
         <f t="shared" si="0"/>
         <v>0.81572510012535737</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
-      <c r="A25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
         <v>24</v>
       </c>
-      <c r="B25">
+      <c r="B26" s="4">
         <f t="shared" si="0"/>
         <v>0.60835131453225522</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
-      <c r="A26">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
         <v>25</v>
       </c>
-      <c r="B26">
+      <c r="B27" s="4">
         <f t="shared" si="0"/>
         <v>0.34663531783502582</v>
       </c>
@@ -926,16 +1001,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -943,7 +1016,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -951,7 +1024,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -959,7 +1032,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -967,7 +1040,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>

</xml_diff>